<commit_message>
Guardar archivos a Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/Data.xlsx
+++ b/src/test/resources/Data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\RetoFalabella\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{B7157E8E-4E00-4074-8724-2DC992446F4F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{5FAF1E7A-1460-4124-B1E7-72A393725B6D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{9204AB78-06FD-44B8-AA9E-84E9497D74B8}" yWindow="-120"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Search</t>
   </si>
@@ -36,73 +36,34 @@
     <t>Validation</t>
   </si>
   <si>
-    <t>Televisor</t>
-  </si>
-  <si>
-    <t>HYUNDAI
-Google Tv Hyundai Smart 42 Fhd Comando De. Voz
-Por Hyundai Electronics
-$ 949.900
--32%
-$ 999.900
-$ 1.390.900
-Agregar al Carro
-Patrocinado</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
     <t>SAMSUNG
-Televisor Samsung 70 pulgadas Crystal UHD 4K HDR Smart TV UN70CU8000
-Por Falabella
+Televisor Samsung 43 pulgadas Crystal UHD 4K HDR Smart TV UN43CU8000
+Por Marketplace
 (10)
-Tamaño de la pantalla: 70 pulgadas
+Tamaño de la pantalla: 43 pulgadas
 Tecnología: Crystal UHD
-Modelo: UN70CU8000KXZL
+Modelo: UN43CU8000KXZL
 Tasa de refresco: 60Hz
 Garantía del proveedor: 1 año
-$ 2.999.900
--40%
-$ 3.199.900
-$ 4.999.900
+$ 1.499.900
+-44%
+$ 2.699.900
+Retiro en Tienda 3hrs
 Agregar al Carro</t>
   </si>
   <si>
-    <t>TCL
-Televisor TCL 43 Pulgadas LED 4K Ultra HD Smart TV
-Por Falabella
-(6)
-Tamaño de la pantalla: 43 pulgadas
-Tecnología: LED
-Modelo: 43P635
-Tasa de refresco: 60Hz
-Garantía del proveedor: 2 años
-$ 1.299.900
--41%
-$ 2.199.900
-Agregar al Carro</t>
+    <t>Balon</t>
+  </si>
+  <si>
+    <t>GOLTY
+BALÓN DE FÚTBOL PARA NIÑOS GOLTY DINO No4...
+Por E &amp; M S.a</t>
   </si>
   <si>
     <t>2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>SAMSUNG
-Televisor Samsung 55 Pulgadas NEO QLED 4K Ultra HD Smart TV QN55QN85
-Por Falabella
-(11)
-Tamaño de la pantalla: 55 pulgadas
-Tecnología: NEO QLED
-Modelo: QN55QN85BAKXZL
-Tasa de refresco: 120Hz
-Garantía del proveedor: 1 año
-$ 3.739.900
--47%
-$ 6.999.900
-Agregar al Carro</t>
   </si>
 </sst>
 </file>
@@ -465,7 +426,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,13 +448,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Refinamiento de codigo y mejora en las questions
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/Data.xlsx
+++ b/src/test/resources/Data/Data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>Search</t>
   </si>
@@ -64,6 +64,27 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>MONKEY BRANDS
+Balón de Microfútbol No. 3 Blanco
+Por Monkey Market</t>
+  </si>
+  <si>
+    <t>MOLTEN
+BALON PARA BALONCESTO BF1601...
+Por Ramse Importaciones</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>MOLTEN
+Balón de baloncesto molten b7 g2000 12 paneles
+Por One Zone Sport Sas</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -451,10 +472,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>